<commit_message>
No changes to DB
</commit_message>
<xml_diff>
--- a/data/final_assignments.xlsx
+++ b/data/final_assignments.xlsx
@@ -506,12 +506,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>M. Cenk Gursoy</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Jay Henderson</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Jay Henderson</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Bing Dong</t>
         </is>
       </c>
     </row>
@@ -626,12 +626,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Chikukuri Monhan</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Farzana Rahman</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>M. Cenk Gursoy</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Jay Henderson</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Farzana Rahman</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Bing Dong</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Qinru Qiu</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Shalabh Maroo</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Shalabh Maroo</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Farzana Rahman</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>C.Y. Roger Chen</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Shalabh Maroo</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Ashok Sangani</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Chikukuri Monhan</t>
         </is>
       </c>
     </row>
@@ -1106,12 +1106,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Bing Dong</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Gabriel Silva De Oliveira</t>
         </is>
       </c>
     </row>
@@ -1226,12 +1226,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Jay Henderson</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Amit Sanyal</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Gabriel Silva De Oliveira</t>
+          <t>Mary Beth Monroe</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Bing Dong</t>
         </is>
       </c>
     </row>
@@ -1426,12 +1426,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -1466,12 +1466,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Ian Hosein</t>
+          <t>Ashok Sangani</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Endadul Hoque</t>
+          <t>Amit Sanyal</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Amit Sanyal</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>Ashok Sangani</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Younes Radi</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -1586,12 +1586,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Gabriel Silva De Oliveira</t>
+          <t>M. Cenk Gursoy</t>
         </is>
       </c>
     </row>
@@ -1626,12 +1626,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>John F. Dannenhoffer</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -1666,12 +1666,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
     </row>
@@ -1706,12 +1706,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Shalabh Maroo</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>
@@ -1746,12 +1746,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Amit Sanyal</t>
+          <t>Pankaj Jha</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Shikha Nangia</t>
         </is>
       </c>
     </row>
@@ -1786,12 +1786,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>M. Cenk Gursoy</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Gabriel Silva De Oliveira</t>
         </is>
       </c>
     </row>
@@ -1826,12 +1826,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Shikha Nangia</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>C.Y. Roger Chen</t>
         </is>
       </c>
     </row>
@@ -1866,12 +1866,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Ian Hosein</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Min Liu</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -1906,12 +1906,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
+          <t>Anupam Pandey</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
           <t>John F. Dannenhoffer</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>M. Cenk Gursoy</t>
         </is>
       </c>
     </row>
@@ -1946,12 +1946,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Chikukuri Monhan</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Pankaj Jha</t>
+          <t>Joao Paulo Marum</t>
         </is>
       </c>
     </row>
@@ -1986,12 +1986,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Endadul Hoque</t>
         </is>
       </c>
     </row>
@@ -2026,12 +2026,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ian Hosein</t>
+          <t>C.Y. Roger Chen</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Qinru Qiu</t>
         </is>
       </c>
     </row>
@@ -2066,12 +2066,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Younes Radi</t>
+          <t>Gabriel Silva De Oliveira</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Endadul Hoque</t>
+          <t>Mary Beth Monroe</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Shikha Nangia</t>
         </is>
       </c>
     </row>
@@ -2146,12 +2146,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Shikha Nangia</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Pankaj Jha</t>
         </is>
       </c>
     </row>
@@ -2186,12 +2186,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Mary Beth Monroe</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Min Liu</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -2266,12 +2266,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pankaj Jha</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -2306,12 +2306,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>Jay Henderson</t>
         </is>
       </c>
     </row>
@@ -2346,12 +2346,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
+          <t>Anupam Pandey</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
           <t>Baris Salman</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Shalabh Maroo</t>
         </is>
       </c>
     </row>
@@ -2386,12 +2386,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Bing Dong</t>
         </is>
       </c>
     </row>
@@ -2426,12 +2426,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Chikukuri Monhan</t>
         </is>
       </c>
     </row>
@@ -2466,12 +2466,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>C.Y. Roger Chen</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2506,12 +2506,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>John F. Dannenhoffer</t>
+          <t>Ashok Sangani</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2546,12 +2546,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Era Jain</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>M. Cenk Gursoy</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -2586,12 +2586,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Joao Paulo Marum</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>C.Y. Roger Chen</t>
+          <t>Shikha Nangia</t>
         </is>
       </c>
     </row>
@@ -2626,12 +2626,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Chikukuri Monhan</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Qinru Qiu</t>
         </is>
       </c>
     </row>
@@ -2666,12 +2666,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Younes Radi</t>
         </is>
       </c>
     </row>
@@ -2706,12 +2706,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Ian Hosein</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Shalabh Maroo</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Ian Hosein</t>
         </is>
       </c>
     </row>
@@ -2786,12 +2786,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
     </row>
@@ -2826,12 +2826,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Mary Beth Monroe</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Joao Paulo Marum</t>
         </is>
       </c>
     </row>
@@ -2866,12 +2866,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Ashok Sangani</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -2906,12 +2906,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -2946,12 +2946,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Bing Dong</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Mary Beth Monroe</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2986,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Endadul Hoque</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Qinru Qiu</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>
@@ -3026,12 +3026,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Min Liu</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Younes Radi</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -3066,12 +3066,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>John F. Dannenhoffer</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Pankaj Jha</t>
         </is>
       </c>
     </row>
@@ -3106,12 +3106,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Farzana Rahman</t>
         </is>
       </c>
     </row>
@@ -3146,12 +3146,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -3186,12 +3186,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
DB Handler changed: better matching
</commit_message>
<xml_diff>
--- a/data/final_assignments.xlsx
+++ b/data/final_assignments.xlsx
@@ -506,12 +506,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>M. Cenk Gursoy</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Jay Henderson</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Jay Henderson</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -626,12 +626,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Anupam Pandey</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Yiyang Sun</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Shalabh Maroo</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Shalabh Maroo</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Farzana Rahman</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>C.Y. Roger Chen</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Shalabh Maroo</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -1106,12 +1106,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>Yaoying Wu</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>Zhenyu Gan</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Gabriel Silva De Oliveira</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
     </row>
@@ -1226,12 +1226,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Amit Sanyal</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -1426,12 +1426,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>
@@ -1466,12 +1466,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Amit Sanyal</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Younes Radi</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>M. Cenk Gursoy</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>
@@ -1626,12 +1626,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>John F. Dannenhoffer</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>M. Cenk Gursoy</t>
         </is>
       </c>
     </row>
@@ -1666,12 +1666,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -1706,12 +1706,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -1746,12 +1746,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pankaj Jha</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -1786,12 +1786,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>M. Cenk Gursoy</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Gabriel Silva De Oliveira</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
     </row>
@@ -1826,12 +1826,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>C.Y. Roger Chen</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1866,12 +1866,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
+          <t>Senem Velipasalar</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
           <t>Ben Akih-Kumgeh</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>John F. Dannenhoffer</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -1946,12 +1946,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Senem Velipasalar</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Endadul Hoque</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -2026,12 +2026,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>C.Y. Roger Chen</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Qinru Qiu</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Gabriel Silva De Oliveira</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2106,12 +2106,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -2146,12 +2146,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Pankaj Jha</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2186,12 +2186,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Min Liu</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -2266,12 +2266,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Baris Salman</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -2306,12 +2306,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Jay Henderson</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2386,12 +2386,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -2426,12 +2426,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -2466,12 +2466,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -2506,12 +2506,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Min Liu</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
     </row>
@@ -2546,12 +2546,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2586,12 +2586,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Shikha Nangia</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2626,12 +2626,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Chikukuri Monhan</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Qinru Qiu</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -2666,12 +2666,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Younes Radi</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -2706,12 +2706,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Ian Hosein</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Sucheta Soundarajan</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Ian Hosein</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -2786,12 +2786,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -2826,12 +2826,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Joao Paulo Marum</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -2866,12 +2866,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Ashok Sangani</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -2906,12 +2906,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Yi Zheng</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2946,12 +2946,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Mary Beth Monroe</t>
+          <t>Baris Salman</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2986,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Endadul Hoque</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Bing Dong</t>
         </is>
       </c>
     </row>
@@ -3066,12 +3066,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>John F. Dannenhoffer</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Pankaj Jha</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -3106,12 +3106,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Min Liu</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Farzana Rahman</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
     </row>
@@ -3146,12 +3146,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
     </row>
@@ -3186,12 +3186,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Bing Dong</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
DB Handler changed: better matching. Max 6 respected
</commit_message>
<xml_diff>
--- a/data/final_assignments.xlsx
+++ b/data/final_assignments.xlsx
@@ -591,7 +591,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -826,12 +826,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>Yuzhe Tang</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Senem Velipasalar</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Anupam Pandey</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Yaoying Wu</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>Yuzhe Tang</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
           <t>Senem Velipasalar</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -1226,12 +1226,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
+          <t>Era Jain</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>Zhenyu Gan</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -1266,12 +1266,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
+          <t>Elizabeth Carter</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
           <t>Yaoying Wu</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>M. Cenk Gursoy</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -1746,12 +1746,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Jeongmin Ahn</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Senem Velipasalar</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -1826,12 +1826,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1986,12 +1986,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Zhenyu Gan</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Anupam Pandey</t>
+          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2066,12 +2066,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -2186,12 +2186,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Ben Akih-Kumgeh</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
+          <t>Zhenyu Gan</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
           <t>Yuzhe Tang</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Zhenyu Gan</t>
         </is>
       </c>
     </row>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -2306,12 +2306,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2346,12 +2346,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Jeongmin Ahn</t>
+          <t>Anupam Pandey</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Baris Salman</t>
+          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -2386,12 +2386,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -2426,12 +2426,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
+          <t>Senem Velipasalar</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
           <t>Nadeem Ghani</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Yi Zheng</t>
         </is>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2546,12 +2546,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2666,12 +2666,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Zhenyu Gan</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Nadeem Ghani</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
     </row>
@@ -2706,12 +2706,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Min Liu</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Sucheta Soundarajan</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Yi Zheng</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -2786,12 +2786,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -2826,12 +2826,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Ben Akih-Kumgeh</t>
         </is>
       </c>
     </row>
@@ -2866,12 +2866,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
+          <t>Jeongmin Ahn</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
           <t>Anupam Pandey</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Yaoying Wu</t>
         </is>
       </c>
     </row>
@@ -2906,12 +2906,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
+          <t>Nadeem Ghani</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
           <t>Yi Zheng</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2986,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Yuzhe Tang</t>
+          <t>Jason Pollack</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Svetoslava Todorova</t>
+          <t>Nadeem Ghani</t>
         </is>
       </c>
     </row>
@@ -3026,12 +3026,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
+          <t>Ben Akih-Kumgeh</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
           <t>Ruth Chen</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Bing Dong</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3071,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Yuzhe Tang</t>
         </is>
       </c>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Jason Pollack</t>
+          <t>Svetoslava Todorova</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -3186,12 +3186,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Bing Dong</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
DB Handler changed: better matching. Max 6 respected, Storing match rate
</commit_message>
<xml_diff>
--- a/data/final_assignments.xlsx
+++ b/data/final_assignments.xlsx
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Jesse Q. Bond</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Wanliang Shan</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Era Jain</t>
         </is>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Wanliang Shan</t>
         </is>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Yiyang Sun</t>
         </is>
       </c>
     </row>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Yiyang Sun</t>
+          <t>Jesse Q. Bond</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Era Jain</t>
+          <t>Ruth Chen</t>
         </is>
       </c>
     </row>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Ruth Chen</t>
+          <t>Elizabeth Carter</t>
         </is>
       </c>
     </row>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Elizabeth Carter</t>
+          <t>Zhen Ma</t>
         </is>
       </c>
     </row>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Zhen Ma</t>
+          <t>Era Jain</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">

</xml_diff>